<commit_message>
add create excel logmovement
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS21"/>
+  <dimension ref="A1:AS22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -556,7 +556,7 @@
         <v/>
       </c>
       <c r="F2" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G2" t="str">
         <v/>
@@ -607,10 +607,10 @@
         <v/>
       </c>
       <c r="W2" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X2" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y2" t="str">
         <v/>
@@ -693,7 +693,7 @@
         <v/>
       </c>
       <c r="F3" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G3" t="str">
         <v/>
@@ -744,10 +744,10 @@
         <v/>
       </c>
       <c r="W3" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X3" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y3" t="str">
         <v/>
@@ -830,7 +830,7 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G4" t="str">
         <v/>
@@ -881,10 +881,10 @@
         <v/>
       </c>
       <c r="W4" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X4" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y4" t="str">
         <v/>
@@ -967,7 +967,7 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G5" t="str">
         <v/>
@@ -1015,10 +1015,10 @@
         <v/>
       </c>
       <c r="W5" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X5" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y5" t="str">
         <v/>
@@ -1101,7 +1101,7 @@
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G6" t="str">
         <v/>
@@ -1152,10 +1152,10 @@
         <v/>
       </c>
       <c r="W6" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X6" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y6" t="str">
         <v/>
@@ -1238,7 +1238,7 @@
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G7" t="str">
         <v/>
@@ -1289,10 +1289,10 @@
         <v/>
       </c>
       <c r="W7" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X7" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y7" t="str">
         <v/>
@@ -1375,7 +1375,7 @@
         <v/>
       </c>
       <c r="F8" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G8" t="str">
         <v/>
@@ -1423,10 +1423,10 @@
         <v/>
       </c>
       <c r="W8" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X8" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y8" t="str">
         <v/>
@@ -1509,7 +1509,7 @@
         <v/>
       </c>
       <c r="F9" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G9" t="str">
         <v/>
@@ -1557,10 +1557,10 @@
         <v/>
       </c>
       <c r="W9" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X9" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y9" t="str">
         <v/>
@@ -1643,7 +1643,7 @@
         <v/>
       </c>
       <c r="F10" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G10" t="str">
         <v/>
@@ -1691,10 +1691,10 @@
         <v/>
       </c>
       <c r="W10" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X10" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y10" t="str">
         <v/>
@@ -1777,7 +1777,7 @@
         <v/>
       </c>
       <c r="F11" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G11" t="str">
         <v/>
@@ -1828,10 +1828,10 @@
         <v/>
       </c>
       <c r="W11" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X11" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y11" t="str">
         <v/>
@@ -1914,7 +1914,7 @@
         <v/>
       </c>
       <c r="F12" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G12" t="str">
         <v/>
@@ -1965,10 +1965,10 @@
         <v/>
       </c>
       <c r="W12" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X12" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y12" t="str">
         <v/>
@@ -2051,7 +2051,7 @@
         <v/>
       </c>
       <c r="F13" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G13" t="str">
         <v/>
@@ -2102,10 +2102,10 @@
         <v/>
       </c>
       <c r="W13" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X13" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y13" t="str">
         <v/>
@@ -2188,7 +2188,7 @@
         <v/>
       </c>
       <c r="F14" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G14" t="str">
         <v/>
@@ -2236,10 +2236,10 @@
         <v/>
       </c>
       <c r="W14" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X14" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y14" t="str">
         <v/>
@@ -2322,7 +2322,7 @@
         <v/>
       </c>
       <c r="F15" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G15" t="str">
         <v/>
@@ -2373,10 +2373,10 @@
         <v/>
       </c>
       <c r="W15" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X15" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y15" t="str">
         <v/>
@@ -2459,7 +2459,7 @@
         <v/>
       </c>
       <c r="F16" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G16" t="str">
         <v/>
@@ -2510,10 +2510,10 @@
         <v/>
       </c>
       <c r="W16" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X16" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y16" t="str">
         <v/>
@@ -2596,7 +2596,7 @@
         <v/>
       </c>
       <c r="F17" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G17" t="str">
         <v/>
@@ -2647,10 +2647,10 @@
         <v/>
       </c>
       <c r="W17" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X17" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y17" t="str">
         <v/>
@@ -2733,7 +2733,7 @@
         <v/>
       </c>
       <c r="F18" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G18" t="str">
         <v/>
@@ -2784,10 +2784,10 @@
         <v/>
       </c>
       <c r="W18" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X18" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y18" t="str">
         <v/>
@@ -2870,7 +2870,7 @@
         <v/>
       </c>
       <c r="F19" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G19" t="str">
         <v/>
@@ -2921,10 +2921,10 @@
         <v>proCode1</v>
       </c>
       <c r="W19" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X19" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y19" t="str">
         <v/>
@@ -3007,7 +3007,7 @@
         <v/>
       </c>
       <c r="F20" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G20" t="str">
         <v/>
@@ -3058,10 +3058,10 @@
         <v>proCode2</v>
       </c>
       <c r="W20" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X20" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y20" t="str">
         <v/>
@@ -3144,7 +3144,7 @@
         <v/>
       </c>
       <c r="F21" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="G21" t="str">
         <v/>
@@ -3195,10 +3195,10 @@
         <v>proCode3</v>
       </c>
       <c r="W21" t="str">
-        <v>20277</v>
+        <v>saleCode=20277</v>
       </c>
       <c r="X21" t="str">
-        <v>20250417</v>
+        <v>20250418</v>
       </c>
       <c r="Y21" t="str">
         <v/>
@@ -3261,12 +3261,149 @@
         <v/>
       </c>
       <c r="AS21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>V01000390</v>
+      </c>
+      <c r="B22" t="str">
+        <v>F10</v>
+      </c>
+      <c r="C22" t="str">
+        <v>215</v>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <v>20250418</v>
+      </c>
+      <c r="G22" t="str">
+        <v>test</v>
+      </c>
+      <c r="H22" t="str">
+        <v>6804132150016</v>
+      </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <v>10010101018</v>
+      </c>
+      <c r="K22" t="str">
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <v>PCS</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>109</v>
+      </c>
+      <c r="O22" t="str">
+        <v>PCS</v>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
+      <c r="Q22" t="str">
+        <v/>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" t="str">
+        <v/>
+      </c>
+      <c r="U22" t="str">
+        <v/>
+      </c>
+      <c r="V22" t="str">
+        <v/>
+      </c>
+      <c r="W22" t="str">
+        <v>saleCode=20277</v>
+      </c>
+      <c r="X22" t="str">
+        <v>20250418</v>
+      </c>
+      <c r="Y22" t="str">
+        <v/>
+      </c>
+      <c r="Z22" t="str">
+        <v/>
+      </c>
+      <c r="AA22" t="str">
+        <v/>
+      </c>
+      <c r="AB22" t="str">
+        <v/>
+      </c>
+      <c r="AC22" t="str">
+        <v/>
+      </c>
+      <c r="AD22" t="str">
+        <v/>
+      </c>
+      <c r="AE22" t="str">
+        <v/>
+      </c>
+      <c r="AF22" t="str">
+        <v/>
+      </c>
+      <c r="AG22" t="str">
+        <v/>
+      </c>
+      <c r="AH22" t="str">
+        <v/>
+      </c>
+      <c r="AI22" t="str">
+        <v/>
+      </c>
+      <c r="AJ22" t="str">
+        <v/>
+      </c>
+      <c r="AK22" t="str">
+        <v/>
+      </c>
+      <c r="AL22" t="str">
+        <v/>
+      </c>
+      <c r="AM22" t="str">
+        <v/>
+      </c>
+      <c r="AN22" t="str">
+        <v/>
+      </c>
+      <c r="AO22" t="str">
+        <v/>
+      </c>
+      <c r="AP22" t="str">
+        <v/>
+      </c>
+      <c r="AQ22" t="str">
+        <v/>
+      </c>
+      <c r="AR22" t="str">
+        <v/>
+      </c>
+      <c r="AS22" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AS21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AS22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>